<commit_message>
Rasterización del modelo de predicción
</commit_message>
<xml_diff>
--- a/Analisis_vibrio/DatosTotal.xlsx
+++ b/Analisis_vibrio/DatosTotal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Vibrio\Vibrio_ExpPacifico2021\Analisis_vibrio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian Bermúdez R\Documents\Vibrio_ExpPacifico2021\Analisis_vibrio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBBBF16A-BF49-4AE7-AA4E-6E88565F5918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F124A5D6-BD09-4018-BB58-581C58E3437D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosVibrio" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="PCA" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DatosTotal!$A$1:$O$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DatosTotal!$A$1:$Q$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DatosVibrio!$A$1:$D$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">VibrioTotal2!$A$1:$AA$25</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="95">
   <si>
     <t>A01A</t>
   </si>
@@ -692,7 +692,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5361,2321 +5361,2535 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8BBA67-66DB-41D9-9F0D-5BA50E31A4D6}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T37"/>
+      <selection activeCell="B1" sqref="B1:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>74</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>87</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>71</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>88</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>93</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>94</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>89</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>2.8492999999999999</v>
+      </c>
+      <c r="C2">
+        <v>-78.2226</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>0.06</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>0.38</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.13</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>8.41</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.85</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>8.2899999999999991</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>7.73</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>13</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>49.85</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>27.596299999999999</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>29.113099999999999</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>1018.1609999999999</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>977</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>67.580399999999997</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>75.945999999999998</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>17</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>13.2392655093982</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3">
+        <v>2.8492999999999999</v>
+      </c>
+      <c r="C3">
+        <v>-78.2226</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>0.2</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>0.66</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.06</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>24.29</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>1.7</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>8.25</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>7.52</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>4</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>14.67</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>28.718399999999999</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>28.353200000000001</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>1017.3105</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>5383</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>100.3146</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>796.9701</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>39</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>11.2051448155995</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>2.81677</v>
+      </c>
+      <c r="C4">
+        <v>-78.222499999999997</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>0.13</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>0.7</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0.06</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>11.22</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.83</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>8.26</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>7.41</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>8.5</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>24</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>27.912600000000001</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>26.0307</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>1015.8097</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>860</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>188.06370000000001</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>365.44310000000002</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>16</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>12.976933390088201</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
       <c r="B5">
+        <v>2.81677</v>
+      </c>
+      <c r="C5">
+        <v>-78.222499999999997</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>0.27</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>0.46</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.13</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>16.760000000000002</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>1.86</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>8.25</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>7.19</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>5.5</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>18.25</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>30.017099999999999</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>26.0718</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>1015.046</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>5142</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>73.651300000000006</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>919.15679999999998</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>24</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>7.1762781707641201</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
+        <v>2.7842199999999999</v>
+      </c>
+      <c r="C6">
+        <v>-78.222499999999997</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>0.49</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>1.51</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.24</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>25.38</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>0.5</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>8.2799999999999994</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>7.81</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>2.5</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>17.3</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>26.765799999999999</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>26.665099999999999</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>1016.5468</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>1128</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>204.47929999999999</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>77.410499999999999</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>12</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>4.6858106571012899</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
+        <v>2.7842199999999999</v>
+      </c>
+      <c r="C7">
+        <v>-78.222499999999997</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>1.06</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.23</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>19.84</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>1.6</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>8.23</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>6.48</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>2</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>28</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>26.563400000000001</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>12.991099999999999</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>1006.6156999999999</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>3440</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>29.313800000000001</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>626.22770000000003</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>25</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>10.2381400463115</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
+        <v>2.7516699999999998</v>
+      </c>
+      <c r="C8">
+        <v>-78.222399999999993</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>0.15</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>0.47</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>0.19</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>8.32</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>0.5</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>8.23</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>7.58</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>6</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>23.05</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>27.048500000000001</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>29.019400000000001</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>1018.3309</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>530</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>201.16560000000001</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>563.69529999999997</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>8</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>5.9929326866963004</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
       <c r="B9">
+        <v>2.7516699999999998</v>
+      </c>
+      <c r="C9">
+        <v>-78.222399999999993</v>
+      </c>
+      <c r="D9">
         <v>0</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>0.5</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>1.06</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>0.33</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>17.21</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>1.5</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>8.1999999999999993</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>6.39</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>2</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>28.3</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>27.290700000000001</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>30.119399999999999</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>1019.0881000000001</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>3707</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>51.047600000000003</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>18.936699999999998</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>27</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>12.3482601125635</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
+        <v>2.7191200000000002</v>
+      </c>
+      <c r="C10">
+        <v>-78.222399999999993</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>0.54</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>1.1299999999999999</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>0.26</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>19.21</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>8.16</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>6.84</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>1.6</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>25.85</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>26.788499999999999</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>28.358599999999999</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>1017.9209</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>1208</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>222.6885</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>230.3124</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>16</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>6.9578182753211504</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
+        <v>2.7191200000000002</v>
+      </c>
+      <c r="C11">
+        <v>-78.222399999999993</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>0.64</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>1.24</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>0.37</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>20.3</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>3</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>8.19</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>6.31</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>1.5</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>35.950000000000003</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>27.4224</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>29.5563</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>1018.581</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>3274</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>27.097899999999999</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>753.34680000000003</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>26</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>9.7245059557585503</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
       <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
+        <v>2.6865700000000001</v>
+      </c>
+      <c r="C12">
+        <v>-78.222399999999993</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>0.77</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>1.17</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>0.38</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>25.2</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>4.5999999999999996</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>8.14</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>6.33</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>1.8</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>37.75</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>26.8459</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>29.022099999999998</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>1018.3412</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>12372</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>17.563099999999999</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>100.2808</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>29</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>7.6336739765203196</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
       <c r="B13">
+        <v>2.6865700000000001</v>
+      </c>
+      <c r="C13">
+        <v>-78.222399999999993</v>
+      </c>
+      <c r="D13">
         <v>0</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>0.92</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>0.2</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>28.01</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>4.7300000000000004</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>8.16</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>6.16</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>2</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>49.9</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>27.129100000000001</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>25.168099999999999</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>1015.4325</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>2978</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>28.984500000000001</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>1024.3429000000001</v>
       </c>
-      <c r="S13">
+      <c r="U13">
         <v>19</v>
       </c>
-      <c r="T13">
+      <c r="V13">
         <v>7.0661398699279401</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
       <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
+        <v>2.78403</v>
+      </c>
+      <c r="C14">
+        <v>-78.400499999999994</v>
       </c>
       <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>0.05</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>0.27</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>0.06</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>5.41</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>0.79</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>8.2100000000000009</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>8.06</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>7</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>20.6</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>27.511700000000001</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>26.697199999999999</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>1016.352</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>2507</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>291.47789999999998</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>922.98469999999998</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>23</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <v>11.4183003516355</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
       <c r="B15">
+        <v>2.78403</v>
+      </c>
+      <c r="C15">
+        <v>-78.400499999999994</v>
+      </c>
+      <c r="D15">
         <v>0</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15">
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>0.11</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>0.13</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>24.02</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>1.57</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>8.24</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>7.6</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>2.5</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>27.85</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>27.235600000000002</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>11.8956</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>1005.5034000000001</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <v>1724</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>53.926600000000001</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <v>929.86369999999999</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>21</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>10.203512083009899</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
+        <v>2.7515000000000001</v>
+      </c>
+      <c r="C16">
+        <v>-78.400499999999994</v>
       </c>
       <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16">
         <v>0.09</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>1.03</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>0.13</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>14.58</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>0.74</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>8.2200000000000006</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>7.63</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>3.5</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>21.85</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>24.667000000000002</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>26.2349</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>1016.8337</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>2238</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>274.53590000000003</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>440.35090000000002</v>
       </c>
-      <c r="S16">
+      <c r="U16">
         <v>26</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>8.8538105129371605</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
       <c r="B17">
+        <v>2.7515000000000001</v>
+      </c>
+      <c r="C17">
+        <v>-78.400499999999994</v>
+      </c>
+      <c r="D17">
         <v>0</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17">
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>2</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>0.23</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>33.270000000000003</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>1.47</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>8.18</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>7.25</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>1.2</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>34.9</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <v>27.973199999999999</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>16.303799999999999</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>1008.5972</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <v>2788</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>7.1646999999999998</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>851.29600000000005</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>32</v>
       </c>
-      <c r="T17">
+      <c r="V17">
         <v>16.5564903509588</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
       <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
+        <v>2.71895</v>
+      </c>
+      <c r="C18">
+        <v>-78.400400000000005</v>
       </c>
       <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>0.13</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>1.54</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>0.2</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>12.58</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>0.69</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>8.24</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>7.29</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>6</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>27.2</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>27.2636</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>29.4739</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>1018.4902</v>
       </c>
-      <c r="P18">
+      <c r="R18">
         <v>360</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>183.9555</v>
       </c>
-      <c r="R18">
+      <c r="T18">
         <v>611.70719999999994</v>
       </c>
-      <c r="S18">
+      <c r="U18">
         <v>12</v>
       </c>
-      <c r="T18">
+      <c r="V18">
         <v>8.2194763616186695</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
       <c r="B19">
+        <v>2.71895</v>
+      </c>
+      <c r="C19">
+        <v>-78.400400000000005</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19">
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>0.23</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>2.15</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>0.34</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>32.549999999999997</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>0.94</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>8.16</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>6.84</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
         <v>37.1</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>27.924299999999999</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>23.940200000000001</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>1014.189</v>
       </c>
-      <c r="P19">
+      <c r="R19">
         <v>1657</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>12.5106</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <v>238.29849999999999</v>
       </c>
-      <c r="S19">
+      <c r="U19">
         <v>21</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>12.990082281696001</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
       <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
+        <v>2.6863999999999999</v>
+      </c>
+      <c r="C20">
+        <v>-78.400400000000005</v>
       </c>
       <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>0.05</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>0.36</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>0.13</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>3.51</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>0.32</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>8.18</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>7.19</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>1.8</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>24.1</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>26.689499999999999</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <v>18.835599999999999</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>1010.8592</v>
       </c>
-      <c r="P20">
+      <c r="R20">
         <v>1422</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <v>490.10169999999999</v>
       </c>
-      <c r="R20">
+      <c r="T20">
         <v>122.3394</v>
       </c>
-      <c r="S20">
+      <c r="U20">
         <v>29</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>21.415062874403599</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
       <c r="B21">
+        <v>2.6863999999999999</v>
+      </c>
+      <c r="C21">
+        <v>-78.400400000000005</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>0.32</v>
-      </c>
-      <c r="E21">
-        <v>4.09</v>
+      <c r="E21" s="1">
+        <v>1</v>
       </c>
       <c r="F21">
         <v>0.32</v>
       </c>
       <c r="G21">
+        <v>4.09</v>
+      </c>
+      <c r="H21">
+        <v>0.32</v>
+      </c>
+      <c r="I21">
         <v>78.47</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>1.34</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>7.95</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>6.48</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>0.8</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>50.38</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>27.168800000000001</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>17.771699999999999</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>1009.7976</v>
       </c>
-      <c r="P21">
+      <c r="R21">
         <v>6384</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>5.5461999999999998</v>
       </c>
-      <c r="R21">
+      <c r="T21">
         <v>160.3466</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <v>35</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>6.0063640841186903</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
       <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
+        <v>2.6538499999999998</v>
+      </c>
+      <c r="C22">
+        <v>-78.400400000000005</v>
       </c>
       <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22">
         <v>0.1</v>
       </c>
-      <c r="E22">
+      <c r="G22">
         <v>0.7</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <v>0.23</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>11.58</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>0.73</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>8.16</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>6.78</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>0.8</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>34.950000000000003</v>
       </c>
-      <c r="M22">
+      <c r="O22">
         <v>26.9316</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>22.1402</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>1013.3003</v>
       </c>
-      <c r="P22">
+      <c r="R22">
         <v>3067</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>29.547000000000001</v>
       </c>
-      <c r="R22">
+      <c r="T22">
         <v>638.18100000000004</v>
       </c>
-      <c r="S22">
+      <c r="U22">
         <v>37</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <v>20.2373039292894</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
       <c r="B23">
+        <v>2.6538499999999998</v>
+      </c>
+      <c r="C23">
+        <v>-78.400400000000005</v>
+      </c>
+      <c r="D23">
         <v>0</v>
       </c>
-      <c r="C23" s="1">
+      <c r="E23" s="1">
         <v>0</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <v>0.33</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>3.98</v>
       </c>
-      <c r="F23">
+      <c r="H23">
         <v>0.35</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>71.3</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>1.57</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>7.96</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>6.06</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>0.8</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>72</v>
       </c>
-      <c r="M23">
+      <c r="O23">
         <v>27.4788</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>19.7624</v>
       </c>
-      <c r="O23">
+      <c r="Q23">
         <v>1011.1396999999999</v>
       </c>
-      <c r="P23">
+      <c r="R23">
         <v>5106</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <v>6.4946999999999999</v>
       </c>
-      <c r="R23">
+      <c r="T23">
         <v>85.451400000000007</v>
       </c>
-      <c r="S23">
+      <c r="U23">
         <v>25</v>
       </c>
-      <c r="T23">
+      <c r="V23">
         <v>7.6201193986274598</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
       <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
+        <v>2.6213000000000002</v>
+      </c>
+      <c r="C24">
+        <v>-78.400300000000001</v>
       </c>
       <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <v>0.15</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <v>1.1499999999999999</v>
       </c>
-      <c r="F24">
+      <c r="H24">
         <v>0.42</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <v>16.850000000000001</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>0.86</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>8.14</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>6.62</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>0.6</v>
       </c>
-      <c r="L24">
+      <c r="N24">
         <v>53.53</v>
       </c>
-      <c r="M24">
+      <c r="O24">
         <v>27.663599999999999</v>
       </c>
-      <c r="N24">
+      <c r="P24">
         <v>27.815300000000001</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <v>1017.1047</v>
       </c>
-      <c r="P24">
+      <c r="R24">
         <v>5686</v>
       </c>
-      <c r="Q24">
+      <c r="S24">
         <v>47.531500000000001</v>
       </c>
-      <c r="R24">
+      <c r="T24">
         <v>1191.8986</v>
       </c>
-      <c r="S24">
+      <c r="U24">
         <v>30</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <v>11.7198947558038</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
       <c r="B25">
+        <v>2.6213000000000002</v>
+      </c>
+      <c r="C25">
+        <v>-78.400300000000001</v>
+      </c>
+      <c r="D25">
         <v>0</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25">
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25">
         <v>0.37</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>4.3099999999999996</v>
       </c>
-      <c r="F25">
+      <c r="H25">
         <v>0.62</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <v>77.47</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>1.38</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>7.87</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>5.87</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>0.6</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>77</v>
       </c>
-      <c r="M25">
+      <c r="O25">
         <v>26.890999999999998</v>
       </c>
-      <c r="N25">
+      <c r="P25">
         <v>12.9757</v>
       </c>
-      <c r="O25">
+      <c r="Q25">
         <v>1006.2509</v>
       </c>
-      <c r="P25">
+      <c r="R25">
         <v>7562</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <v>0.50780000000000003</v>
       </c>
-      <c r="R25">
+      <c r="T25">
         <v>30.1282</v>
       </c>
-      <c r="S25">
+      <c r="U25">
         <v>12</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <v>2.3014494384537501</v>
       </c>
     </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
       <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="s">
+        <v>2.8329399999999998</v>
+      </c>
+      <c r="C26">
+        <v>-78.319699999999997</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D26">
+      <c r="F26">
         <v>0.05</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>0.36</v>
       </c>
-      <c r="F26">
+      <c r="H26">
         <v>0.11</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>11.4</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>1.1299999999999999</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>8.2200000000000006</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>7.66</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>10.5</v>
       </c>
-      <c r="L26">
+      <c r="N26">
         <v>16.3</v>
       </c>
-      <c r="M26">
+      <c r="O26">
         <v>27.270900000000001</v>
       </c>
-      <c r="N26">
+      <c r="P26">
         <v>26.5318</v>
       </c>
-      <c r="O26">
+      <c r="Q26">
         <v>1016.3019</v>
       </c>
-      <c r="P26">
+      <c r="R26">
         <v>1774</v>
       </c>
-      <c r="Q26">
+      <c r="S26">
         <v>55.790599999999998</v>
       </c>
-      <c r="R26">
+      <c r="T26">
         <v>389.55439999999999</v>
       </c>
-      <c r="S26">
+      <c r="U26">
         <v>17</v>
       </c>
-      <c r="T26">
+      <c r="V26">
         <v>4.46800637327709</v>
       </c>
     </row>
-    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
       <c r="B27">
+        <v>2.8329399999999998</v>
+      </c>
+      <c r="C27">
+        <v>-78.319699999999997</v>
+      </c>
+      <c r="D27">
         <v>0</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>0.06</v>
       </c>
-      <c r="E27">
+      <c r="G27">
         <v>0.19</v>
       </c>
-      <c r="F27">
+      <c r="H27">
         <v>0.09</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>6.86</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>0.81</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>8.2200000000000006</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>7.05</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>8.5</v>
       </c>
-      <c r="L27">
+      <c r="N27">
         <v>18.12</v>
       </c>
-      <c r="M27">
+      <c r="O27">
         <v>26.9163</v>
       </c>
-      <c r="N27">
+      <c r="P27">
         <v>0.35010000000000002</v>
       </c>
-      <c r="O27">
+      <c r="Q27">
         <v>996.97670000000005</v>
       </c>
-      <c r="P27">
+      <c r="R27">
         <v>760</v>
       </c>
-      <c r="Q27">
+      <c r="S27">
         <v>580.96130000000005</v>
       </c>
-      <c r="R27">
+      <c r="T27">
         <v>959.22400000000005</v>
       </c>
-      <c r="S27">
+      <c r="U27">
         <v>14</v>
       </c>
-      <c r="T27">
+      <c r="V27">
         <v>9.5836864428994097</v>
       </c>
     </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
       <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
+        <v>2.8003999999999998</v>
+      </c>
+      <c r="C28">
+        <v>-78.319599999999994</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D28">
+      <c r="F28">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E28">
+      <c r="G28">
         <v>0.6</v>
       </c>
-      <c r="F28">
+      <c r="H28">
         <v>0.1</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>10.95</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>1.07</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <v>8.2100000000000009</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>7.37</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>5</v>
       </c>
-      <c r="L28">
+      <c r="N28">
         <v>19.95</v>
       </c>
-      <c r="M28">
+      <c r="O28">
         <v>27.4268</v>
       </c>
-      <c r="N28">
+      <c r="P28">
         <v>25.475999999999999</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <v>1015.4554000000001</v>
       </c>
-      <c r="P28">
+      <c r="R28">
         <v>2147</v>
       </c>
-      <c r="Q28">
+      <c r="S28">
         <v>150.55670000000001</v>
       </c>
-      <c r="R28">
+      <c r="T28">
         <v>474.1669</v>
       </c>
-      <c r="S28">
+      <c r="U28">
         <v>11</v>
       </c>
-      <c r="T28">
+      <c r="V28">
         <v>2.4954089429057098</v>
       </c>
     </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
       <c r="B29">
+        <v>2.8003999999999998</v>
+      </c>
+      <c r="C29">
+        <v>-78.319599999999994</v>
+      </c>
+      <c r="D29">
         <v>0</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E29">
+      <c r="G29">
         <v>0.36</v>
       </c>
-      <c r="F29">
+      <c r="H29">
         <v>0.06</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>10.039999999999999</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>0.84</v>
       </c>
-      <c r="I29">
+      <c r="K29">
         <v>8.17</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>6.93</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>6</v>
       </c>
-      <c r="L29">
+      <c r="N29">
         <v>31.3</v>
       </c>
-      <c r="M29">
+      <c r="O29">
         <v>28.392099999999999</v>
       </c>
-      <c r="N29">
+      <c r="P29">
         <v>19.476199999999999</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <v>1010.6994999999999</v>
       </c>
-      <c r="P29">
+      <c r="R29">
         <v>1760</v>
       </c>
-      <c r="Q29">
+      <c r="S29">
         <v>49.831299999999999</v>
       </c>
-      <c r="R29">
+      <c r="T29">
         <v>784.0548</v>
       </c>
-      <c r="S29">
+      <c r="U29">
         <v>18</v>
       </c>
-      <c r="T29">
+      <c r="V29">
         <v>8.2348149206617194</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
       <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1">
+        <v>2.7678500000000001</v>
+      </c>
+      <c r="C30">
+        <v>-78.319599999999994</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
         <v>0</v>
       </c>
-      <c r="D30">
+      <c r="F30">
         <v>0.11</v>
       </c>
-      <c r="E30">
+      <c r="G30">
         <v>0.64</v>
       </c>
-      <c r="F30">
+      <c r="H30">
         <v>0.19</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <v>10.77</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>0.75</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <v>8.19</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <v>7.04</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>2.5</v>
       </c>
-      <c r="L30">
+      <c r="N30">
         <v>27.15</v>
       </c>
-      <c r="M30">
+      <c r="O30">
         <v>25.649899999999999</v>
       </c>
-      <c r="N30">
+      <c r="P30">
         <v>7.1950000000000003</v>
       </c>
-      <c r="O30">
+      <c r="Q30">
         <v>1002.5278</v>
       </c>
-      <c r="P30">
+      <c r="R30">
         <v>5688</v>
       </c>
-      <c r="Q30">
+      <c r="S30">
         <v>371.7627</v>
       </c>
-      <c r="R30">
+      <c r="T30">
         <v>1001.8804</v>
       </c>
-      <c r="S30">
+      <c r="U30">
         <v>27</v>
       </c>
-      <c r="T30">
+      <c r="V30">
         <v>4.3648430636908699</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
       <c r="B31">
+        <v>2.7678500000000001</v>
+      </c>
+      <c r="C31">
+        <v>-78.319599999999994</v>
+      </c>
+      <c r="D31">
         <v>0</v>
       </c>
-      <c r="C31" s="1">
+      <c r="E31" s="1">
         <v>0</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <v>0.45</v>
       </c>
-      <c r="E31">
+      <c r="G31">
         <v>1.21</v>
       </c>
-      <c r="F31">
+      <c r="H31">
         <v>0.36</v>
       </c>
-      <c r="G31">
+      <c r="I31">
         <v>27.28</v>
       </c>
-      <c r="H31">
+      <c r="J31">
         <v>1.23</v>
       </c>
-      <c r="I31">
+      <c r="K31">
         <v>8.1199999999999992</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>6.29</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>0.9</v>
       </c>
-      <c r="L31">
+      <c r="N31">
         <v>35.799999999999997</v>
       </c>
-      <c r="M31">
+      <c r="O31">
         <v>25.745100000000001</v>
       </c>
-      <c r="N31">
+      <c r="P31">
         <v>1.6371</v>
       </c>
-      <c r="O31">
+      <c r="Q31">
         <v>998.30039999999997</v>
       </c>
-      <c r="P31">
+      <c r="R31">
         <v>9568</v>
       </c>
-      <c r="Q31">
+      <c r="S31">
         <v>10.357200000000001</v>
       </c>
-      <c r="R31">
+      <c r="T31">
         <v>497.58229999999998</v>
       </c>
-      <c r="S31">
+      <c r="U31">
         <v>39</v>
       </c>
-      <c r="T31">
+      <c r="V31">
         <v>7.8813995867641298</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
       <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
+        <v>2.7353000000000001</v>
+      </c>
+      <c r="C32">
+        <v>-78.319500000000005</v>
       </c>
       <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32">
         <v>0.09</v>
       </c>
-      <c r="E32">
+      <c r="G32">
         <v>0.87</v>
       </c>
-      <c r="F32">
+      <c r="H32">
         <v>0.33</v>
       </c>
-      <c r="G32">
+      <c r="I32">
         <v>12.67</v>
       </c>
-      <c r="H32">
+      <c r="J32">
         <v>0.73</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>8.16</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <v>6.85</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>2.5</v>
       </c>
-      <c r="L32">
+      <c r="N32">
         <v>22.6</v>
       </c>
-      <c r="M32">
+      <c r="O32">
         <v>26.984100000000002</v>
       </c>
-      <c r="N32">
+      <c r="P32">
         <v>24.479900000000001</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>1014.9614</v>
       </c>
-      <c r="P32">
+      <c r="R32">
         <v>5650</v>
       </c>
-      <c r="Q32">
+      <c r="S32">
         <v>1913.1839</v>
       </c>
-      <c r="R32">
+      <c r="T32">
         <v>3070.9694</v>
       </c>
-      <c r="S32">
+      <c r="U32">
         <v>39</v>
       </c>
-      <c r="T32">
+      <c r="V32">
         <v>10.4143351185784</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
       <c r="B33">
+        <v>2.7353000000000001</v>
+      </c>
+      <c r="C33">
+        <v>-78.319500000000005</v>
+      </c>
+      <c r="D33">
         <v>0</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33">
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>0.69</v>
       </c>
-      <c r="E33">
+      <c r="G33">
         <v>2.17</v>
       </c>
-      <c r="F33">
+      <c r="H33">
         <v>0.35</v>
       </c>
-      <c r="G33">
+      <c r="I33">
         <v>42.35</v>
       </c>
-      <c r="H33">
+      <c r="J33">
         <v>2.39</v>
       </c>
-      <c r="I33">
+      <c r="K33">
         <v>8.1</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <v>5.91</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <v>0.75</v>
       </c>
-      <c r="L33">
+      <c r="N33">
         <v>42.1</v>
       </c>
-      <c r="M33">
+      <c r="O33">
         <v>27.644200000000001</v>
       </c>
-      <c r="N33">
+      <c r="P33">
         <v>26.170300000000001</v>
       </c>
-      <c r="O33">
+      <c r="Q33">
         <v>1015.8712</v>
       </c>
-      <c r="P33">
+      <c r="R33">
         <v>5408</v>
       </c>
-      <c r="Q33">
+      <c r="S33">
         <v>59.764800000000001</v>
       </c>
-      <c r="R33">
+      <c r="T33">
         <v>612.51700000000005</v>
       </c>
-      <c r="S33">
+      <c r="U33">
         <v>27</v>
       </c>
-      <c r="T33">
+      <c r="V33">
         <v>8.0767894080307308</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
       <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
+        <v>2.70275</v>
+      </c>
+      <c r="C34">
+        <v>-78.319500000000005</v>
       </c>
       <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <v>0.06</v>
       </c>
-      <c r="E34">
+      <c r="G34">
         <v>0.53</v>
       </c>
-      <c r="F34">
+      <c r="H34">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G34">
+      <c r="I34">
         <v>9.41</v>
       </c>
-      <c r="H34">
+      <c r="J34">
         <v>1.1399999999999999</v>
       </c>
-      <c r="I34">
+      <c r="K34">
         <v>8.1199999999999992</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>6.7</v>
       </c>
-      <c r="K34">
+      <c r="M34">
         <v>2.5</v>
       </c>
-      <c r="L34">
+      <c r="N34">
         <v>77.75</v>
       </c>
-      <c r="M34">
+      <c r="O34">
         <v>27.790299999999998</v>
       </c>
-      <c r="N34">
+      <c r="P34">
         <v>8.4428999999999998</v>
       </c>
-      <c r="O34">
+      <c r="Q34">
         <v>1002.6861</v>
       </c>
-      <c r="P34">
+      <c r="R34">
         <v>18353</v>
       </c>
-      <c r="Q34">
+      <c r="S34">
         <v>332.10500000000002</v>
       </c>
-      <c r="R34">
+      <c r="T34">
         <v>1386.7113999999999</v>
       </c>
-      <c r="S34">
+      <c r="U34">
         <v>41</v>
       </c>
-      <c r="T34">
+      <c r="V34">
         <v>11.025364299403201</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>61</v>
       </c>
       <c r="B35">
+        <v>2.70275</v>
+      </c>
+      <c r="C35">
+        <v>-78.319500000000005</v>
+      </c>
+      <c r="D35">
         <v>0</v>
       </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35">
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <v>0.84</v>
       </c>
-      <c r="E35">
+      <c r="G35">
         <v>1.49</v>
       </c>
-      <c r="F35">
+      <c r="H35">
         <v>0.91</v>
       </c>
-      <c r="G35">
+      <c r="I35">
         <v>45.98</v>
       </c>
-      <c r="H35">
+      <c r="J35">
         <v>3.64</v>
       </c>
-      <c r="I35">
+      <c r="K35">
         <v>8.0399999999999991</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <v>5.6</v>
       </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35">
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
         <v>87.55</v>
       </c>
-      <c r="M35">
+      <c r="O35">
         <v>26.4223</v>
       </c>
-      <c r="N35">
+      <c r="P35">
         <v>4.3041</v>
       </c>
-      <c r="O35">
+      <c r="Q35">
         <v>1000.0697</v>
       </c>
-      <c r="P35">
+      <c r="R35">
         <v>6766</v>
       </c>
-      <c r="Q35">
+      <c r="S35">
         <v>4.5347999999999997</v>
       </c>
-      <c r="R35">
+      <c r="T35">
         <v>347.84969999999998</v>
       </c>
-      <c r="S35">
+      <c r="U35">
         <v>42</v>
       </c>
-      <c r="T35">
+      <c r="V35">
         <v>14.6413983524731</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>62</v>
       </c>
       <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1</v>
+        <v>2.6701999999999999</v>
+      </c>
+      <c r="C36">
+        <v>-78.319500000000005</v>
       </c>
       <c r="D36">
-        <v>0.25</v>
-      </c>
-      <c r="E36">
-        <v>2.2799999999999998</v>
+        <v>1</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
       </c>
       <c r="F36">
         <v>0.25</v>
       </c>
       <c r="G36">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="H36">
+        <v>0.25</v>
+      </c>
+      <c r="I36">
         <v>44.44</v>
       </c>
-      <c r="H36">
+      <c r="J36">
         <v>1.57</v>
       </c>
-      <c r="I36">
+      <c r="K36">
         <v>8.0299999999999994</v>
       </c>
-      <c r="J36">
+      <c r="L36">
         <v>6.12</v>
       </c>
-      <c r="K36">
+      <c r="M36">
         <v>2.5</v>
       </c>
-      <c r="L36">
+      <c r="N36">
         <v>160.97</v>
       </c>
-      <c r="M36">
+      <c r="O36">
         <v>27.64</v>
       </c>
-      <c r="N36">
+      <c r="P36">
         <v>10.684699999999999</v>
       </c>
-      <c r="O36">
+      <c r="Q36">
         <v>1004.4749</v>
       </c>
-      <c r="P36">
+      <c r="R36">
         <v>29298</v>
       </c>
-      <c r="Q36">
+      <c r="S36">
         <v>19.608799999999999</v>
       </c>
-      <c r="R36">
+      <c r="T36">
         <v>588.48490000000004</v>
       </c>
-      <c r="S36">
+      <c r="U36">
         <v>42</v>
       </c>
-      <c r="T36">
+      <c r="V36">
         <v>8.0195667808350297</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>62</v>
       </c>
       <c r="B37">
+        <v>2.6701999999999999</v>
+      </c>
+      <c r="C37">
+        <v>-78.319500000000005</v>
+      </c>
+      <c r="D37">
         <v>0</v>
       </c>
-      <c r="C37" s="1">
+      <c r="E37" s="1">
         <v>0</v>
       </c>
-      <c r="D37">
+      <c r="F37">
         <v>0.73</v>
       </c>
-      <c r="E37">
+      <c r="G37">
         <v>2.46</v>
       </c>
-      <c r="F37">
+      <c r="H37">
         <v>0.47</v>
       </c>
-      <c r="G37">
+      <c r="I37">
         <v>44.98</v>
       </c>
-      <c r="H37">
+      <c r="J37">
         <v>4.99</v>
       </c>
-      <c r="I37">
+      <c r="K37">
         <v>8.02</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <v>5.41</v>
       </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37">
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
         <v>188.05</v>
       </c>
-      <c r="M37">
+      <c r="O37">
         <v>25.470400000000001</v>
       </c>
-      <c r="N37">
+      <c r="P37">
         <v>0.40150000000000002</v>
       </c>
-      <c r="O37">
+      <c r="Q37">
         <v>997.41229999999996</v>
       </c>
-      <c r="P37">
+      <c r="R37">
         <v>14414</v>
       </c>
-      <c r="Q37">
+      <c r="S37">
         <v>49.240900000000003</v>
       </c>
-      <c r="R37">
+      <c r="T37">
         <v>1772.8036</v>
       </c>
-      <c r="S37">
+      <c r="U37">
         <v>49</v>
       </c>
-      <c r="T37">
+      <c r="V37">
         <v>12.628623950165901</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O37" xr:uid="{9D8BBA67-66DB-41D9-9F0D-5BA50E31A4D6}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="0"/>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q37" xr:uid="{9D8BBA67-66DB-41D9-9F0D-5BA50E31A4D6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>